<commit_message>
some design  & not-even-working table pages method
</commit_message>
<xml_diff>
--- a/importData.xlsx
+++ b/importData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\FIT\XML subject\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54E8E34-7568-4345-8D87-2175FB810C7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585D44C5-EC01-4346-8DA8-16E457B1B843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,42 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test1 desc</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>test4</t>
-  </si>
-  <si>
-    <t>test5</t>
-  </si>
-  <si>
-    <t>test6</t>
-  </si>
-  <si>
-    <t>test2 desc</t>
-  </si>
-  <si>
-    <t>test3 desc</t>
-  </si>
-  <si>
-    <t>test4 desc</t>
-  </si>
-  <si>
-    <t>test5 desc</t>
-  </si>
-  <si>
-    <t>test6 desc</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+  <si>
+    <t>Plate</t>
+  </si>
+  <si>
+    <t>30kg - Steel stainless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10kg - stainless steel </t>
+  </si>
+  <si>
+    <t>Bench for crunches</t>
+  </si>
+  <si>
+    <t>Leather bench made specifically for crunches and similar activities</t>
+  </si>
+  <si>
+    <t>Gripper</t>
+  </si>
+  <si>
+    <t>5kg resistance</t>
+  </si>
+  <si>
+    <t>10kg resistance</t>
+  </si>
+  <si>
+    <t>Water bottle</t>
+  </si>
+  <si>
+    <t>Plastic water bottle with clapper cap</t>
   </si>
 </sst>
 </file>
@@ -381,13 +375,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="57.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -395,7 +390,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>85.5</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -403,13 +398,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -417,21 +412,21 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>85.12</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -439,21 +434,21 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>35.5</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>12.95</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>